<commit_message>
Updating testing results and PMS1003 code
</commit_message>
<xml_diff>
--- a/Testing/Ash Chamber Sensor Testing/Testing 16 Aug/OPC and PMS Chamber testing 16Aug 2nd Run.xlsx
+++ b/Testing/Ash Chamber Sensor Testing/Testing 16 Aug/OPC and PMS Chamber testing 16Aug 2nd Run.xlsx
@@ -641,7 +641,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -655,7 +655,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-NZ"/>
-              <a:t>AC Fine Test Dust Test</a:t>
+              <a:t>AC Fine Test Dust Testing</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -673,7 +673,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -7788,7 +7788,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -7801,7 +7801,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-NZ" sz="1200"/>
+                  <a:rPr lang="en-NZ"/>
                   <a:t>Time (s)</a:t>
                 </a:r>
               </a:p>
@@ -7820,7 +7820,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -7858,7 +7858,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -7905,7 +7905,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -7918,14 +7918,9 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-NZ" sz="1200"/>
-                  <a:t>Concentration</a:t>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>Concentration (mg/m^3)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-NZ" sz="1200" baseline="0"/>
-                  <a:t> (mg/m^3)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-NZ" sz="1200"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -7942,7 +7937,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -7980,7 +7975,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -8022,7 +8017,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -8062,7 +8057,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1400"/>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -8096,7 +8091,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -8110,13 +8105,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-NZ"/>
-              <a:t>OPCN2 Parcticle</a:t>
+              <a:t>OPCN2 Parcticle Distribution over AC Test Dust Test</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-NZ" baseline="0"/>
-              <a:t> Distribution over AC Test Dust Test</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-NZ"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -8133,7 +8123,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -15023,7 +15013,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -15036,7 +15026,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-NZ" sz="1200"/>
+                  <a:rPr lang="en-NZ"/>
                   <a:t>Time (s)</a:t>
                 </a:r>
               </a:p>
@@ -15055,7 +15045,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -15093,7 +15083,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -15143,7 +15133,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -15156,7 +15146,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-NZ" sz="1200"/>
+                  <a:rPr lang="en-NZ"/>
                   <a:t>Concentration (mg/m^3)</a:t>
                 </a:r>
               </a:p>
@@ -15175,7 +15165,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -15207,7 +15197,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -15249,7 +15239,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -15289,7 +15279,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1400"/>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -16408,15 +16398,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>771524</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>47623</xdr:rowOff>
+      <xdr:colOff>733424</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>104773</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>104774</xdr:rowOff>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -16425,8 +16415,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13392149" y="619123"/>
-          <a:ext cx="3829051" cy="5962651"/>
+          <a:off x="13354049" y="485773"/>
+          <a:ext cx="3829051" cy="6534152"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16475,7 +16465,15 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-NZ" sz="1400" u="none" baseline="0"/>
-            <a:t>OPCN2 was run without the housing, hence no constricting of the outlet.</a:t>
+            <a:t>OPCN2 was </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1400" b="1" u="none" baseline="0"/>
+            <a:t>run without the housing</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1400" u="none" baseline="0"/>
+            <a:t>, hence no constricting of the outlet.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -16534,8 +16532,17 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-NZ" sz="1400" baseline="0"/>
-            <a:t> it stopped logging briefly. Data from this sensor seems quite erratic on first inspection.</a:t>
+            <a:t> it stopped logging briefly. </a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1400" b="1" baseline="0"/>
+            <a:t>Data from this sensor seems quite erratic on first inspection</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1400" b="0" baseline="0"/>
+            <a:t>. To be expected when cheaper.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-NZ" sz="1400" baseline="0"/>
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-NZ" sz="1400" baseline="0"/>
@@ -16551,8 +16558,29 @@
         </a:p>
         <a:p>
           <a:r>
+            <a:rPr lang="en-NZ" sz="1400" b="1" u="none" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Blower was not on to clean lenses!!</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-NZ" sz="1400" u="sng" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
             <a:rPr lang="en-NZ" sz="1400" u="none" baseline="0"/>
-            <a:t>Opacity meter was set with density factor same as with OPCN2 and PMS1003, 1310 kg/m^3 - as calculated for our ash (but not necessarily same for AC test dust).</a:t>
+            <a:t>Opacity meter was set with </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1400" b="1" u="none" baseline="0"/>
+            <a:t>density factor </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1400" u="none" baseline="0"/>
+            <a:t>same as with OPCN2 and PMS1003, 1310 kg/m^3 - as calculated for our ash (but not necessarily same for AC test dust).</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -16570,16 +16598,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>666749</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>219074</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16940,7 +16968,7 @@
   <dimension ref="A1:P593"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S36" sqref="S36"/>
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32113,7 +32141,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V19" sqref="V19"/>
+      <selection activeCell="W17" sqref="W17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>